<commit_message>
Correct the data sheets
</commit_message>
<xml_diff>
--- a/data/exercice 1.xlsx
+++ b/data/exercice 1.xlsx
@@ -1,15 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b04d825435d036ce/Documents/Prevision/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_BCE6ADEF3DCE0DAD053D26BDD880207D3996D314" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91738906-1825-4C8C-AC46-36B3436AF452}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="6855" windowHeight="4380"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -93,8 +97,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,13 +135,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -175,7 +187,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -209,6 +221,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -243,9 +256,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -418,16 +432,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="X1" sqref="X1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +515,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -575,7 +589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -649,7 +663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -723,7 +737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
@@ -797,7 +811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8</v>
       </c>
@@ -871,7 +885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>9</v>
       </c>
@@ -945,7 +959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>10</v>
       </c>
@@ -1019,7 +1033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>11</v>
       </c>
@@ -1093,7 +1107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>12</v>
       </c>
@@ -1167,7 +1181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>15</v>
       </c>
@@ -1241,7 +1255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>16</v>
       </c>
@@ -1315,7 +1329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>17</v>
       </c>
@@ -1389,7 +1403,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>19</v>
       </c>
@@ -1463,7 +1477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>20</v>
       </c>
@@ -1537,7 +1551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>21</v>
       </c>
@@ -1611,7 +1625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>22</v>
       </c>
@@ -1685,7 +1699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>23</v>
       </c>
@@ -1759,7 +1773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>24</v>
       </c>
@@ -1833,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>25</v>
       </c>
@@ -1907,7 +1921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>26</v>
       </c>
@@ -1981,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>27</v>
       </c>
@@ -2055,7 +2069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>28</v>
       </c>
@@ -2129,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:24">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>29</v>
       </c>
@@ -2203,7 +2217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:24">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>31</v>
       </c>
@@ -2277,7 +2291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:24">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>32</v>
       </c>
@@ -2351,7 +2365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:24">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>34</v>
       </c>
@@ -2425,7 +2439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:24">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>35</v>
       </c>
@@ -2499,7 +2513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:24">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>36</v>
       </c>
@@ -2573,7 +2587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:24">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>37</v>
       </c>
@@ -2647,7 +2661,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:24">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>38</v>
       </c>
@@ -2721,7 +2735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:24">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>39</v>
       </c>
@@ -2795,7 +2809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:24">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>40</v>
       </c>
@@ -2869,7 +2883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:24">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>41</v>
       </c>
@@ -2943,7 +2957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:24">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>43</v>
       </c>
@@ -3014,7 +3028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:24">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>44</v>
       </c>
@@ -3088,7 +3102,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:24">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>46</v>
       </c>
@@ -3162,7 +3176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:24">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>50</v>
       </c>
@@ -3236,7 +3250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:24">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>51</v>
       </c>
@@ -3310,7 +3324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:24">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>52</v>
       </c>
@@ -3384,7 +3398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:24">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>54</v>
       </c>
@@ -3458,7 +3472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:24">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>55</v>
       </c>
@@ -3532,7 +3546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:24">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>57</v>
       </c>
@@ -3606,7 +3620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:24">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>58</v>
       </c>
@@ -3680,7 +3694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:24">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>60</v>
       </c>
@@ -3754,7 +3768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:24">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>62</v>
       </c>
@@ -3828,7 +3842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:24">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>64</v>
       </c>
@@ -3902,7 +3916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:24">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>65</v>
       </c>
@@ -3976,7 +3990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:24">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>67</v>
       </c>
@@ -4050,7 +4064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:24">
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>68</v>
       </c>
@@ -4124,7 +4138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:24">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>70</v>
       </c>
@@ -4198,7 +4212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:24">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>72</v>
       </c>
@@ -4272,7 +4286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:24">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>75</v>
       </c>
@@ -4346,7 +4360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:24">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>76</v>
       </c>
@@ -4420,7 +4434,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:24">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>78</v>
       </c>
@@ -4494,7 +4508,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:24">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>79</v>
       </c>
@@ -4568,7 +4582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:24">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>80</v>
       </c>
@@ -4642,7 +4656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:24">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>81</v>
       </c>
@@ -4716,7 +4730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:24">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>83</v>
       </c>
@@ -4790,7 +4804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:24">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>85</v>
       </c>
@@ -4864,7 +4878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:24">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>87</v>
       </c>
@@ -4938,7 +4952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:24">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>88</v>
       </c>
@@ -5012,7 +5026,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:24">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>90</v>
       </c>
@@ -5086,7 +5100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:24">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>91</v>
       </c>
@@ -5160,7 +5174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:24">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>92</v>
       </c>
@@ -5234,7 +5248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:24">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>95</v>
       </c>
@@ -5308,7 +5322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:24">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>96</v>
       </c>
@@ -5382,7 +5396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:24">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>97</v>
       </c>
@@ -5456,7 +5470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:24">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>105</v>
       </c>
@@ -5530,7 +5544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:24">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>106</v>
       </c>
@@ -5604,7 +5618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:24">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>107</v>
       </c>
@@ -5678,7 +5692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:24">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>108</v>
       </c>
@@ -5752,7 +5766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:24">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>109</v>
       </c>
@@ -5826,7 +5840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:24">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>111</v>
       </c>
@@ -5900,7 +5914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:24">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>113</v>
       </c>
@@ -5974,7 +5988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:24">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>114</v>
       </c>
@@ -6048,7 +6062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:24">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>115</v>
       </c>
@@ -6122,7 +6136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:24">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>117</v>
       </c>
@@ -6196,7 +6210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:24">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>122</v>
       </c>
@@ -6270,7 +6284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:24">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>124</v>
       </c>
@@ -6344,7 +6358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:24">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>135</v>
       </c>
@@ -6418,7 +6432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:24">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>136</v>
       </c>
@@ -6492,7 +6506,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:24">
+    <row r="83" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>137</v>
       </c>
@@ -6566,7 +6580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:24">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>138</v>
       </c>
@@ -6640,7 +6654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:24">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>139</v>
       </c>
@@ -6714,7 +6728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:24">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>140</v>
       </c>
@@ -6788,7 +6802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:24">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>141</v>
       </c>
@@ -6862,7 +6876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:24">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>143</v>
       </c>
@@ -6936,7 +6950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:24">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>144</v>
       </c>
@@ -7010,7 +7024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:24">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>145</v>
       </c>
@@ -7084,7 +7098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:24">
+    <row r="91" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>147</v>
       </c>
@@ -7158,7 +7172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:24">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>148</v>
       </c>
@@ -7235,28 +7249,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>